<commit_message>
simulate invoice in different currency
</commit_message>
<xml_diff>
--- a/docs/accounting/v9-v10/03.1_delete_buy_invoice.xlsx
+++ b/docs/accounting/v9-v10/03.1_delete_buy_invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diako/project/omega/docs/accounting/v9-v10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB791B6-340C-F84E-A945-669E90915CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84468B6-24E0-6B49-B3F4-66FBF001A323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3287,8 +3287,8 @@
   </sheetPr>
   <dimension ref="A1:I143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>

</xml_diff>